<commit_message>
update of euro-cordex simulation table
</commit_message>
<xml_diff>
--- a/euro-cordex-esgf.xlsx
+++ b/euro-cordex-esgf.xlsx
@@ -25962,7 +25962,7 @@
       </c>
       <c r="J788" t="inlineStr">
         <is>
-          <t>['rsds', 'rlds', 'rsus', 'rlus', 'prc', 'sfcWind', 'psl', 'ps', 'pr', 'zmla', 'va100m', 'vas', 'evspsblpot', 'hfss', 'hfls', 'evspsbl', 'mrso', 'mrros', 'huss', 'hurs', 'mrro', 'clt', 'tauv', 'tauu', 'ua100m', 'snm', 'sund', 'snw', 'tas', 'uas', 'ts']</t>
+          <t>['rsds', 'rlds', 'rsus', 'rlus', 'prc', 'sfcWind', 'psl', 'ps', 'pr', 'zmla', 'va100m', 'vas', 'hfss', 'hfls', 'evspsbl', 'mrso', 'mrros', 'huss', 'hurs', 'mrro', 'clt', 'tauv', 'tauu', 'ua100m', 'snm', 'sund', 'snw', 'tas', 'uas', 'ts']</t>
         </is>
       </c>
     </row>
@@ -50594,7 +50594,7 @@
       </c>
       <c r="J1551" t="inlineStr">
         <is>
-          <t>['rsds', 'rlds', 'hfss', 'hfls']</t>
+          <t>['rsds', 'rlds']</t>
         </is>
       </c>
     </row>
@@ -50710,7 +50710,7 @@
       </c>
       <c r="J1555" t="inlineStr">
         <is>
-          <t>['rsds', 'rlds', 'hfss', 'hfls']</t>
+          <t>['rsds', 'rlds']</t>
         </is>
       </c>
     </row>
@@ -50854,7 +50854,7 @@
       </c>
       <c r="J1560" t="inlineStr">
         <is>
-          <t>['rsds', 'rlds', 'hfss', 'hfls']</t>
+          <t>['rsds', 'rlds']</t>
         </is>
       </c>
     </row>

</xml_diff>